<commit_message>
Y1D - MS Assignment Template Update + Add timeline
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockD/MS Assignment Template/ADS&AI Worklog -  Y1D_2022-23_ADSAI.xlsx
+++ b/docs/Year1/BlockD/MS Assignment Template/ADS&AI Worklog -  Y1D_2022-23_ADSAI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Google Drive\BUAS\ADSAI\Teamwork\MS Teams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year1\BlockD\MS Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD9D7E75-34A0-47A7-A521-EE81B1CBABF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8751127-F96C-4D86-9AAC-922883A9EE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Worklog_Tasks&amp;Times'!$A$1:$K$115</definedName>
     <definedName name="Z_8BAC9A6B_5D32_4E8D_967D_E17D357516F8_.wvu.FilterData" localSheetId="0" hidden="1">'Worklog_Tasks&amp;Times'!$A$1:$K$15</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="TODO" guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -30,9 +30,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -704,17 +707,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -727,41 +760,11 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,9 +1182,9 @@
   </sheetPr>
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1234,7 +1237,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="49"/>
@@ -1252,35 +1255,35 @@
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="54"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
@@ -1507,7 +1510,7 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="49"/>
@@ -1525,35 +1528,35 @@
       <c r="A17" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="54"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="54"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="32">
@@ -1780,53 +1783,53 @@
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="54"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
     </row>
     <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="54"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="52"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="54"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
     </row>
     <row r="33" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
@@ -2053,53 +2056,53 @@
       <c r="K43" s="24"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="54"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="52"/>
     </row>
     <row r="45" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="54"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="52"/>
     </row>
     <row r="46" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="54"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="52"/>
     </row>
     <row r="47" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
@@ -2326,53 +2329,53 @@
       <c r="K57" s="24"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="60" t="s">
+      <c r="A58" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="54"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="52"/>
     </row>
     <row r="59" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="52" t="s">
+      <c r="B59" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="53"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="54"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="52"/>
     </row>
     <row r="60" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="53"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="54"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="52"/>
     </row>
     <row r="61" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
@@ -2599,53 +2602,53 @@
       <c r="K71" s="24"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="55" t="s">
+      <c r="A72" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="53"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="53"/>
-      <c r="K72" s="54"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="52"/>
     </row>
     <row r="73" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="53"/>
-      <c r="I73" s="53"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="54"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="51"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="51"/>
+      <c r="J73" s="51"/>
+      <c r="K73" s="52"/>
     </row>
     <row r="74" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B74" s="56" t="s">
+      <c r="B74" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="53"/>
-      <c r="D74" s="53"/>
-      <c r="E74" s="53"/>
-      <c r="F74" s="53"/>
-      <c r="G74" s="53"/>
-      <c r="H74" s="53"/>
-      <c r="I74" s="53"/>
-      <c r="J74" s="53"/>
-      <c r="K74" s="54"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="51"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="51"/>
+      <c r="K74" s="52"/>
     </row>
     <row r="75" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="13">
@@ -2872,53 +2875,53 @@
       <c r="K85" s="24"/>
     </row>
     <row r="86" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="57" t="s">
+      <c r="A86" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B86" s="53"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
-      <c r="G86" s="53"/>
-      <c r="H86" s="53"/>
-      <c r="I86" s="53"/>
-      <c r="J86" s="53"/>
-      <c r="K86" s="54"/>
+      <c r="B86" s="51"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="51"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="51"/>
+      <c r="I86" s="51"/>
+      <c r="J86" s="51"/>
+      <c r="K86" s="52"/>
     </row>
     <row r="87" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="58" t="s">
+      <c r="B87" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C87" s="53"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="53"/>
-      <c r="G87" s="53"/>
-      <c r="H87" s="53"/>
-      <c r="I87" s="53"/>
-      <c r="J87" s="53"/>
-      <c r="K87" s="54"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
+      <c r="E87" s="51"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="51"/>
+      <c r="I87" s="51"/>
+      <c r="J87" s="51"/>
+      <c r="K87" s="52"/>
     </row>
     <row r="88" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="58" t="s">
+      <c r="B88" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="53"/>
-      <c r="D88" s="53"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="53"/>
-      <c r="G88" s="53"/>
-      <c r="H88" s="53"/>
-      <c r="I88" s="53"/>
-      <c r="J88" s="53"/>
-      <c r="K88" s="54"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="51"/>
+      <c r="E88" s="51"/>
+      <c r="F88" s="51"/>
+      <c r="G88" s="51"/>
+      <c r="H88" s="51"/>
+      <c r="I88" s="51"/>
+      <c r="J88" s="51"/>
+      <c r="K88" s="52"/>
     </row>
     <row r="89" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="13">
@@ -3148,22 +3151,22 @@
       <c r="A100" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B100" s="53"/>
-      <c r="C100" s="53"/>
-      <c r="D100" s="53"/>
-      <c r="E100" s="53"/>
-      <c r="F100" s="53"/>
-      <c r="G100" s="53"/>
-      <c r="H100" s="53"/>
-      <c r="I100" s="53"/>
-      <c r="J100" s="53"/>
-      <c r="K100" s="54"/>
+      <c r="B100" s="51"/>
+      <c r="C100" s="51"/>
+      <c r="D100" s="51"/>
+      <c r="E100" s="51"/>
+      <c r="F100" s="51"/>
+      <c r="G100" s="51"/>
+      <c r="H100" s="51"/>
+      <c r="I100" s="51"/>
+      <c r="J100" s="51"/>
+      <c r="K100" s="52"/>
     </row>
     <row r="101" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="48" t="s">
+      <c r="B101" s="62" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="49"/>
@@ -3174,13 +3177,13 @@
       <c r="H101" s="49"/>
       <c r="I101" s="49"/>
       <c r="J101" s="49"/>
-      <c r="K101" s="50"/>
+      <c r="K101" s="63"/>
     </row>
     <row r="102" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="51" t="s">
+      <c r="B102" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C102" s="49"/>
@@ -3191,7 +3194,7 @@
       <c r="H102" s="49"/>
       <c r="I102" s="49"/>
       <c r="J102" s="49"/>
-      <c r="K102" s="50"/>
+      <c r="K102" s="63"/>
     </row>
     <row r="103" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="13">
@@ -3445,7 +3448,7 @@
   <customSheetViews>
     <customSheetView guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:K15" xr:uid="{6E00989B-777E-4C95-BC05-50EAFDBE28ED}">
+      <autoFilter ref="A1:K15" xr:uid="{9C33D27F-4093-4513-91EC-D8805F086D78}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="- Weekplan item 1_x000a_- Weekplan item 2_x000a_- Weekplan item 3_x000a_- etc"/>
@@ -3456,21 +3459,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="24">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="B17:K17"/>
-    <mergeCell ref="B18:K18"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="B59:K59"/>
-    <mergeCell ref="A100:K100"/>
     <mergeCell ref="B101:K101"/>
     <mergeCell ref="B102:K102"/>
     <mergeCell ref="B60:K60"/>
@@ -3480,6 +3468,21 @@
     <mergeCell ref="A86:K86"/>
     <mergeCell ref="B87:K87"/>
     <mergeCell ref="B88:K88"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="B59:K59"/>
+    <mergeCell ref="A100:K100"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="B17:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B14 B17:B28 B33:B42 B47:B56 B61:B70 B75:B84 B89:B98 B103:B112">
     <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Unplanned">
@@ -3748,35 +3751,35 @@
         <v>36</v>
       </c>
       <c r="C10" s="22">
-        <f ca="1">SUM(C3:C9)</f>
+        <f t="shared" ref="C10:J10" ca="1" si="1">SUM(C3:C9)</f>
         <v>0</v>
       </c>
       <c r="D10" s="22">
-        <f>SUM(D3:D9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E10" s="22">
-        <f>SUM(E3:E9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F10" s="22">
-        <f>SUM(F3:F9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G10" s="22">
-        <f>SUM(G3:G9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10" s="22">
-        <f>SUM(H3:H9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="22">
-        <f>SUM(I3:I9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J10" s="22">
-        <f>SUM(J3:J9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="25"/>
@@ -4973,21 +4976,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DB06FA0A2AD4DA488583749EC2534234" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="886b513cfe8a01d235b598bb5d9e3280">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60348849-ecd6-40c5-8069-7b4f665118aa" xmlns:ns3="d3efc331-58f4-463c-b792-81d907c25a2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea6c152a0770c3b66e26597cca1a51d2" ns2:_="" ns3:_="">
     <xsd:import namespace="60348849-ecd6-40c5-8069-7b4f665118aa"/>
@@ -5204,10 +5192,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEA0944-5FCC-4602-BBF4-AB9918BDC47E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="60348849-ecd6-40c5-8069-7b4f665118aa"/>
+    <ds:schemaRef ds:uri="d3efc331-58f4-463c-b792-81d907c25a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5222,5 +5236,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEA0944-5FCC-4602-BBF4-AB9918BDC47E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>